<commit_message>
Se crean nuevas clases para el escenario del portal crm
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:AL34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -565,7 +565,7 @@
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -718,8 +718,9 @@
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
     <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se realiza ajustes en las clases InvetoryAllocaion Action, adicionando el metodo Leave,se ajusta la clase MerchandiseEntryAction implementenado select par las listas desplegables
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PrepaidAutomation\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963C17C9-678A-4E95-9958-C408275BA4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3470" yWindow="3470" windowWidth="21600" windowHeight="11390"/>
+    <workbookView xWindow="4035" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>MSIDN</t>
   </si>
@@ -62,12 +63,6 @@
     <t>http://10.65.45.12:9001/gatewaycbs/BcServicesInt</t>
   </si>
   <si>
-    <t>8957732111198172294</t>
-  </si>
-  <si>
-    <t>3016877411</t>
-  </si>
-  <si>
     <t>URL DB</t>
   </si>
   <si>
@@ -116,34 +111,31 @@
     <t>http://10.65.45.12:9001/gatewaymgint/GatewayMGWSInt</t>
   </si>
   <si>
-    <t>732111198172293</t>
-  </si>
-  <si>
     <t>MSI</t>
   </si>
   <si>
-    <t>732111198172294</t>
-  </si>
-  <si>
-    <t>8957732111198172293</t>
-  </si>
-  <si>
-    <t>8957732111198172292</t>
-  </si>
-  <si>
-    <t>3016876876</t>
-  </si>
-  <si>
-    <t>3016877591</t>
-  </si>
-  <si>
-    <t>732111198172292</t>
+    <t>8957732111198172291</t>
+  </si>
+  <si>
+    <t>8957732111198172290</t>
+  </si>
+  <si>
+    <t>3016875982</t>
+  </si>
+  <si>
+    <t>3016875893</t>
+  </si>
+  <si>
+    <t>732111198172291</t>
+  </si>
+  <si>
+    <t>732111198172290</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -527,21 +519,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:AL34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -575,77 +567,77 @@
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -668,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -676,13 +668,13 @@
         <v>3003324</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -690,35 +682,21 @@
         <v>3003324</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1">
-        <v>3003324</v>
-      </c>
-      <c r="B13" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
se realiza cambio en la clase PrepaidActivationActions para que reciba por parametros los datos del excel y se modifica los metodos del SanitySteps para pasar lo parametros desde el excel
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963C17C9-678A-4E95-9958-C408275BA4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EE003E-B525-48E1-8CD2-021B9076B7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>MSIDN</t>
   </si>
   <si>
-    <t>SERIAL</t>
-  </si>
-  <si>
-    <t>PLU</t>
-  </si>
-  <si>
     <t>URL EPOS</t>
   </si>
   <si>
@@ -114,12 +108,6 @@
     <t>MSI</t>
   </si>
   <si>
-    <t>8957732111198172291</t>
-  </si>
-  <si>
-    <t>8957732111198172290</t>
-  </si>
-  <si>
     <t>3016875982</t>
   </si>
   <si>
@@ -130,6 +118,18 @@
   </si>
   <si>
     <t>732111198172290</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>Cedula Cliente</t>
+  </si>
+  <si>
+    <t>10960370</t>
+  </si>
+  <si>
+    <t>667299000</t>
   </si>
 </sst>
 </file>
@@ -188,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -205,6 +205,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -520,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -538,106 +542,106 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -650,45 +654,59 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
+      <c r="A10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1">
-        <v>3003324</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1">
-        <v>3003324</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se crean nuevas clases para automatizacion de activacion control
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity Ambientes\PrepaidAutomation\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PrepaidAutomation\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EE003E-B525-48E1-8CD2-021B9076B7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>MSIDN</t>
   </si>
@@ -108,18 +107,6 @@
     <t>MSI</t>
   </si>
   <si>
-    <t>3016875982</t>
-  </si>
-  <si>
-    <t>3016875893</t>
-  </si>
-  <si>
-    <t>732111198172291</t>
-  </si>
-  <si>
-    <t>732111198172290</t>
-  </si>
-  <si>
     <t>Vendedor</t>
   </si>
   <si>
@@ -129,13 +116,28 @@
     <t>10960370</t>
   </si>
   <si>
-    <t>667299000</t>
+    <t>12669894</t>
+  </si>
+  <si>
+    <t>828959809</t>
+  </si>
+  <si>
+    <t>3016877411</t>
+  </si>
+  <si>
+    <t>3016876876</t>
+  </si>
+  <si>
+    <t>732111198172294</t>
+  </si>
+  <si>
+    <t>732111198172293</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -523,21 +525,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -655,10 +657,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -669,52 +671,38 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>